<commit_message>
PDF Single Page done DB Structure Change Bill View Logic change
</commit_message>
<xml_diff>
--- a/SQL Tables.xlsx
+++ b/SQL Tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\souri\Documents\Study\College\Old_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3FABBD-88C0-447F-8073-D0C53C7E9C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467A6AC7-FD24-4080-AED3-F23CEA2FF1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="61">
   <si>
     <t>SuppID</t>
   </si>
@@ -200,6 +200,15 @@
   </si>
   <si>
     <t>VARCHAR(50)</t>
+  </si>
+  <si>
+    <t>Dis_per</t>
+  </si>
+  <si>
+    <t>Paid</t>
+  </si>
+  <si>
+    <t>Dis_ru</t>
   </si>
 </sst>
 </file>
@@ -560,7 +569,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -615,9 +624,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -933,36 +939,37 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:J30"/>
+  <dimension ref="B1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="3.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="25.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="19.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="1" customWidth="1"/>
     <col min="6" max="6" width="17.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="15.6640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="12.88671875" style="1" customWidth="1"/>
     <col min="10" max="10" width="39.109375" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="1"/>
+    <col min="11" max="11" width="14.77734375" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="23"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="22"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
@@ -1033,13 +1040,13 @@
     </row>
     <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="8" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="23"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="22"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
@@ -1105,14 +1112,14 @@
     </row>
     <row r="13" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="23"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="22"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
@@ -1154,7 +1161,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" s="9" t="s">
         <v>2</v>
       </c>
@@ -1174,7 +1181,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="11" t="s">
         <v>4</v>
       </c>
@@ -1188,21 +1195,21 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="24" t="s">
+    <row r="19" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="2:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="26"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="25"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" s="17" t="s">
         <v>0</v>
       </c>
@@ -1227,11 +1234,11 @@
       <c r="I21" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="J21" s="20" t="s">
+      <c r="J21" s="19" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="9" t="s">
         <v>16</v>
       </c>
@@ -1256,11 +1263,11 @@
       <c r="I22" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" s="9" t="s">
         <v>2</v>
       </c>
@@ -1289,7 +1296,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:11" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="15" t="s">
         <v>21</v>
       </c>
@@ -1312,23 +1319,24 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="24" t="s">
+    <row r="26" spans="2:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="26"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="22"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B27" s="17" t="s">
         <v>26</v>
       </c>
@@ -1336,28 +1344,31 @@
         <v>27</v>
       </c>
       <c r="D27" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G27" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E27" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="F27" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="G27" s="18" t="s">
-        <v>48</v>
-      </c>
       <c r="H27" s="18" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="I27" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="J27" s="20" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+      <c r="J27" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="K27" s="19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B28" s="9" t="s">
         <v>28</v>
       </c>
@@ -1365,16 +1376,16 @@
         <v>16</v>
       </c>
       <c r="D28" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="H28" s="5" t="s">
         <v>20</v>
@@ -1382,11 +1393,14 @@
       <c r="I28" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J28" s="10" t="s">
+      <c r="J28" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="K28" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="9" t="s">
         <v>2</v>
       </c>
@@ -1411,11 +1425,14 @@
       <c r="I29" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="J29" s="10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J29" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="K29" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="11" t="s">
         <v>4</v>
       </c>
@@ -1426,11 +1443,12 @@
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
-      <c r="H30" s="12" t="s">
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I30" s="12"/>
-      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1438,7 +1456,7 @@
     <mergeCell ref="B14:G14"/>
     <mergeCell ref="B20:J20"/>
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B26:J26"/>
+    <mergeCell ref="B26:K26"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -1472,14 +1490,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="29"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="28"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -1557,17 +1575,17 @@
     </row>
     <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="29"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="28"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
@@ -1683,16 +1701,16 @@
       <c r="A12" s="2"/>
     </row>
     <row r="13" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="29"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="28"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
@@ -1790,13 +1808,13 @@
     </row>
     <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="19" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="23"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="22"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>

</xml_diff>